<commit_message>
Añadir variable de delitos cortos
</commit_message>
<xml_diff>
--- a/datos_limpios/diccionario.xlsx
+++ b/datos_limpios/diccionario.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regis\OneDrive\Documents\GitHub\Intersecta-PJCDMX\datos_limpios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717C2D42-1AD8-4452-BC30-DCAA232A70B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29339D96-60C9-4222-B3FE-326272947EC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24690" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{12D9CC48-F821-4A99-9FCF-43376564107A}"/>
+    <workbookView xWindow="20490" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{12D9CC48-F821-4A99-9FCF-43376564107A}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="199">
   <si>
     <t>materia</t>
   </si>
@@ -448,13 +449,196 @@
   </si>
   <si>
     <t>Asuntos ingresados</t>
+  </si>
+  <si>
+    <t>num_alcaldias_asunto</t>
+  </si>
+  <si>
+    <t>num_consignacion_asunto</t>
+  </si>
+  <si>
+    <t>num_comision_asunto</t>
+  </si>
+  <si>
+    <t>num_realizacion_asunto</t>
+  </si>
+  <si>
+    <t>num_delitos_asuntos</t>
+  </si>
+  <si>
+    <t>num_alcaldias_sitjurid</t>
+  </si>
+  <si>
+    <t>num_consignacion_sitjurid</t>
+  </si>
+  <si>
+    <t>num_comision_sitjurid</t>
+  </si>
+  <si>
+    <t>num_realizacion_sitjurid</t>
+  </si>
+  <si>
+    <t>num_delitos_sitjurid</t>
+  </si>
+  <si>
+    <t>num_alcaldias_alternas</t>
+  </si>
+  <si>
+    <t>num_consignacion_alternas</t>
+  </si>
+  <si>
+    <t>num_comision_alternas</t>
+  </si>
+  <si>
+    <t>num_realizacion_alternas</t>
+  </si>
+  <si>
+    <t>num_delitos_alternas</t>
+  </si>
+  <si>
+    <t>num_alcaldias_cautelares</t>
+  </si>
+  <si>
+    <t>num_consignacion_cautelares</t>
+  </si>
+  <si>
+    <t>num_comision_cautelares</t>
+  </si>
+  <si>
+    <t>num_realizacion_cautelares</t>
+  </si>
+  <si>
+    <t>num_delitos_cautelares</t>
+  </si>
+  <si>
+    <t>num_alcaldias_sentencia</t>
+  </si>
+  <si>
+    <t>num_consignacion_sentencia</t>
+  </si>
+  <si>
+    <t>num_comision_sentencia</t>
+  </si>
+  <si>
+    <t>num_realizacion_sentencia</t>
+  </si>
+  <si>
+    <t>num_delitos_sentencia</t>
+  </si>
+  <si>
+    <t>num_terminacion</t>
+  </si>
+  <si>
+    <t>num_ppo</t>
+  </si>
+  <si>
+    <t>year_asunto</t>
+  </si>
+  <si>
+    <t>year_sitjurid</t>
+  </si>
+  <si>
+    <t>year_alternas</t>
+  </si>
+  <si>
+    <t>year_cautelares</t>
+  </si>
+  <si>
+    <t>month_asunto</t>
+  </si>
+  <si>
+    <t>month_sitjurid</t>
+  </si>
+  <si>
+    <t>month_alternas</t>
+  </si>
+  <si>
+    <t>month_cautelares</t>
+  </si>
+  <si>
+    <t>date_asunto</t>
+  </si>
+  <si>
+    <t>date_sijurid</t>
+  </si>
+  <si>
+    <t>date_alternas</t>
+  </si>
+  <si>
+    <t>date_cautelares</t>
+  </si>
+  <si>
+    <t>date_sentencia</t>
+  </si>
+  <si>
+    <t>sexo_acusada_asunto</t>
+  </si>
+  <si>
+    <t>sexo_acusada_sitjurid</t>
+  </si>
+  <si>
+    <t>sexo_acusada_alternas</t>
+  </si>
+  <si>
+    <t>sexo_acusada_cautelares</t>
+  </si>
+  <si>
+    <t>edad_acusada_asunto</t>
+  </si>
+  <si>
+    <t>edad_acusada_sitjurid</t>
+  </si>
+  <si>
+    <t>edad_acusada_alternas</t>
+  </si>
+  <si>
+    <t>edad_acusada_cautelares</t>
+  </si>
+  <si>
+    <t>con_terminacion</t>
+  </si>
+  <si>
+    <t>tipo_terminacion</t>
+  </si>
+  <si>
+    <t>con_ppo</t>
+  </si>
+  <si>
+    <t>tipo_ppo</t>
+  </si>
+  <si>
+    <t>materia_asunto</t>
+  </si>
+  <si>
+    <t>materia_sitjurid</t>
+  </si>
+  <si>
+    <t>materia_alternas</t>
+  </si>
+  <si>
+    <t>materia_cautelares</t>
+  </si>
+  <si>
+    <t>materia_sentencia</t>
+  </si>
+  <si>
+    <t>c_con_detenido_asunto</t>
+  </si>
+  <si>
+    <t>c_sin_detenido_asunto</t>
+  </si>
+  <si>
+    <t>c_culposo_asunto</t>
+  </si>
+  <si>
+    <t>c_doloso_asunto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +650,24 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -491,11 +693,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7FAC37-4CD9-42F0-A279-56121884172C}">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:A70"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,4 +2067,408 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED863324-4FDB-4C86-B2DB-2D37067E93A9}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>